<commit_message>
Commited new progress in SprintInfo9
</commit_message>
<xml_diff>
--- a/Documentation and designs/Sprint_info/Sprint9.xlsx
+++ b/Documentation and designs/Sprint_info/Sprint9.xlsx
@@ -462,17 +462,7 @@
     <cellStyle name="Accent6" xfId="2" builtinId="49"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <color theme="0"/>
@@ -592,7 +582,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -887,28 +876,28 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -929,11 +918,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="290087704"/>
-        <c:axId val="290088880"/>
+        <c:axId val="297984608"/>
+        <c:axId val="297981080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="290087704"/>
+        <c:axId val="297984608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1036,7 +1025,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="290088880"/>
+        <c:crossAx val="297981080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1044,7 +1033,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="290088880"/>
+        <c:axId val="297981080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1089,7 +1078,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1148,7 +1136,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="290087704"/>
+        <c:crossAx val="297984608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1811,7 +1799,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2216,7 +2204,7 @@
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2611,7 +2599,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G13" s="19"/>
       <c r="H13" s="19"/>
@@ -2619,7 +2607,9 @@
       <c r="J13" s="19"/>
       <c r="K13" s="19"/>
       <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
+      <c r="M13" s="19">
+        <v>1</v>
+      </c>
       <c r="N13" s="19"/>
       <c r="O13" s="19"/>
       <c r="P13" s="19"/>
@@ -2629,7 +2619,7 @@
       <c r="T13" s="19"/>
       <c r="U13" s="19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
@@ -2673,7 +2663,7 @@
       </c>
       <c r="M14" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14" s="2">
         <f t="shared" si="1"/>
@@ -2705,7 +2695,7 @@
       </c>
       <c r="U14" s="2">
         <f t="shared" ref="U14" si="2">E14-SUM(G14:T14)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
@@ -2816,35 +2806,35 @@
       </c>
       <c r="M16" s="2">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N16" s="2">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O16" s="2">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P16" s="2">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q16" s="2">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R16" s="2">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S16" s="2">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T16" s="2">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U16" s="10"/>
     </row>
@@ -2888,39 +2878,39 @@
     <mergeCell ref="B8:B10"/>
   </mergeCells>
   <conditionalFormatting sqref="U14">
-    <cfRule type="cellIs" dxfId="9" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="13" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F10">
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>"To do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U5:U10">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11:F13">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"To do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U11:U13">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Edited Sprint9 info, reassigned tasks
</commit_message>
<xml_diff>
--- a/Documentation and designs/Sprint_info/Sprint9.xlsx
+++ b/Documentation and designs/Sprint_info/Sprint9.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -918,11 +918,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="297984608"/>
-        <c:axId val="297981080"/>
+        <c:axId val="287363856"/>
+        <c:axId val="287368952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="297984608"/>
+        <c:axId val="287363856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1025,7 +1025,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297981080"/>
+        <c:crossAx val="287368952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1033,7 +1033,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297981080"/>
+        <c:axId val="287368952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1136,7 +1136,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="297984608"/>
+        <c:crossAx val="287363856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2204,7 +2204,7 @@
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2421,7 +2421,7 @@
         <v>41</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E8" s="21">
         <v>1</v>
@@ -2454,7 +2454,9 @@
       <c r="C9" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="21"/>
+      <c r="D9" s="21" t="s">
+        <v>9</v>
+      </c>
       <c r="E9" s="21">
         <v>1</v>
       </c>
@@ -2941,7 +2943,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added info about sprint9 progress
</commit_message>
<xml_diff>
--- a/Documentation and designs/Sprint_info/Sprint9.xlsx
+++ b/Documentation and designs/Sprint_info/Sprint9.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -390,7 +390,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -414,6 +414,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -462,7 +465,32 @@
     <cellStyle name="Accent6" xfId="2" builtinId="49"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -888,16 +916,16 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -918,11 +946,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="287363856"/>
-        <c:axId val="287368952"/>
+        <c:axId val="278235440"/>
+        <c:axId val="278235832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="287363856"/>
+        <c:axId val="278235440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1025,7 +1053,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="287368952"/>
+        <c:crossAx val="278235832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1033,7 +1061,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="287368952"/>
+        <c:axId val="278235832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1136,7 +1164,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="287363856"/>
+        <c:crossAx val="278235440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1799,7 +1827,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2132,21 +2160,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="22"/>
+      <c r="C2" s="23"/>
       <c r="D2" s="12" t="s">
         <v>2</v>
       </c>
@@ -2155,10 +2183,10 @@
       <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="23"/>
+      <c r="C3" s="24"/>
       <c r="D3" s="14" t="s">
         <v>8</v>
       </c>
@@ -2167,10 +2195,10 @@
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="23"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="14" t="s">
         <v>5</v>
       </c>
@@ -2179,10 +2207,10 @@
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="24"/>
+      <c r="C5" s="25"/>
       <c r="D5" s="15" t="s">
         <v>11</v>
       </c>
@@ -2204,7 +2232,7 @@
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2305,10 +2333,10 @@
       </c>
     </row>
     <row r="5" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="30">
+      <c r="B5" s="31">
         <v>3</v>
       </c>
       <c r="C5" s="19" t="s">
@@ -2343,8 +2371,8 @@
       </c>
     </row>
     <row r="6" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="29"/>
-      <c r="B6" s="31"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="19" t="s">
         <v>42</v>
       </c>
@@ -2377,8 +2405,8 @@
       </c>
     </row>
     <row r="7" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="29"/>
-      <c r="B7" s="32"/>
+      <c r="A7" s="30"/>
+      <c r="B7" s="33"/>
       <c r="C7" s="19" t="s">
         <v>44</v>
       </c>
@@ -2411,10 +2439,10 @@
       </c>
     </row>
     <row r="8" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="30">
+      <c r="B8" s="31">
         <v>3</v>
       </c>
       <c r="C8" s="21" t="s">
@@ -2427,7 +2455,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G8" s="21"/>
       <c r="H8" s="21"/>
@@ -2439,18 +2467,20 @@
       <c r="N8" s="21"/>
       <c r="O8" s="21"/>
       <c r="P8" s="21"/>
-      <c r="Q8" s="21"/>
+      <c r="Q8" s="21">
+        <v>1</v>
+      </c>
       <c r="R8" s="21"/>
       <c r="S8" s="21"/>
       <c r="T8" s="21"/>
       <c r="U8" s="21">
         <f>E7-SUM(G8:T8)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
       <c r="C9" s="21" t="s">
         <v>42</v>
       </c>
@@ -2460,8 +2490,8 @@
       <c r="E9" s="21">
         <v>1</v>
       </c>
-      <c r="F9" s="21" t="s">
-        <v>40</v>
+      <c r="F9" s="22" t="s">
+        <v>39</v>
       </c>
       <c r="G9" s="21"/>
       <c r="H9" s="21"/>
@@ -2473,27 +2503,31 @@
       <c r="N9" s="21"/>
       <c r="O9" s="21"/>
       <c r="P9" s="21"/>
-      <c r="Q9" s="21"/>
+      <c r="Q9" s="21">
+        <v>1</v>
+      </c>
       <c r="R9" s="21"/>
       <c r="S9" s="21"/>
       <c r="T9" s="21"/>
       <c r="U9" s="21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32"/>
+      <c r="A10" s="33"/>
+      <c r="B10" s="33"/>
       <c r="C10" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="21"/>
+      <c r="D10" s="21" t="s">
+        <v>6</v>
+      </c>
       <c r="E10" s="21">
         <v>1</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G10" s="21"/>
       <c r="H10" s="21"/>
@@ -2509,16 +2543,16 @@
       <c r="R10" s="21"/>
       <c r="S10" s="21"/>
       <c r="T10" s="21"/>
-      <c r="U10" s="21">
-        <f>U9</f>
+      <c r="U10" s="22">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="30">
+      <c r="B11" s="31">
         <v>5</v>
       </c>
       <c r="C11" s="19" t="s">
@@ -2547,14 +2581,14 @@
       <c r="R11" s="19"/>
       <c r="S11" s="19"/>
       <c r="T11" s="19"/>
-      <c r="U11" s="19">
+      <c r="U11" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="29"/>
-      <c r="B12" s="31"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="32"/>
       <c r="C12" s="19" t="s">
         <v>42</v>
       </c>
@@ -2583,14 +2617,14 @@
       <c r="R12" s="19"/>
       <c r="S12" s="19"/>
       <c r="T12" s="19"/>
-      <c r="U12" s="19">
-        <f t="shared" si="0"/>
+      <c r="U12" s="22">
+        <f>U11</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="29"/>
-      <c r="B13" s="32"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="33"/>
       <c r="C13" s="19" t="s">
         <v>44</v>
       </c>
@@ -2619,9 +2653,9 @@
       <c r="R13" s="19"/>
       <c r="S13" s="19"/>
       <c r="T13" s="19"/>
-      <c r="U13" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="U13" s="22">
+        <f>E12-SUM(G13:T13)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
@@ -2681,7 +2715,7 @@
       </c>
       <c r="Q14" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R14" s="2">
         <f t="shared" si="1"/>
@@ -2697,7 +2731,7 @@
       </c>
       <c r="U14" s="2">
         <f t="shared" ref="U14" si="2">E14-SUM(G14:T14)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
@@ -2824,19 +2858,19 @@
       </c>
       <c r="Q16" s="2">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="R16" s="2">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="S16" s="2">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="T16" s="2">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="U16" s="10"/>
     </row>
@@ -2880,40 +2914,35 @@
     <mergeCell ref="B8:B10"/>
   </mergeCells>
   <conditionalFormatting sqref="U14">
-    <cfRule type="cellIs" dxfId="8" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F10">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>"To do"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U5:U10">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
+  <conditionalFormatting sqref="U5:U13">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11:F13">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"To do"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U11:U13">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
-      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations xWindow="491" yWindow="329" count="1">

</xml_diff>

<commit_message>
Entered info about progress in sprint9
</commit_message>
<xml_diff>
--- a/Documentation and designs/Sprint_info/Sprint9.xlsx
+++ b/Documentation and designs/Sprint_info/Sprint9.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Roster" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -148,16 +148,10 @@
     <t>Done</t>
   </si>
   <si>
-    <t>To do</t>
-  </si>
-  <si>
     <t>Find cause</t>
   </si>
   <si>
     <t>Resolve problem</t>
-  </si>
-  <si>
-    <t>In progress</t>
   </si>
   <si>
     <t>Retesting</t>
@@ -390,7 +384,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -414,6 +408,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -465,22 +462,7 @@
     <cellStyle name="Accent6" xfId="2" builtinId="49"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <font>
         <color theme="0"/>
@@ -610,6 +592,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -922,10 +905,10 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -946,11 +929,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="278235440"/>
-        <c:axId val="278235832"/>
+        <c:axId val="287380816"/>
+        <c:axId val="287381208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="278235440"/>
+        <c:axId val="287380816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1053,7 +1036,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="278235832"/>
+        <c:crossAx val="287381208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1061,7 +1044,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="278235832"/>
+        <c:axId val="287381208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1106,6 +1089,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1164,7 +1148,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="278235440"/>
+        <c:crossAx val="287380816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1827,7 +1811,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2160,21 +2144,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="28"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="29"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="23"/>
+      <c r="C2" s="24"/>
       <c r="D2" s="12" t="s">
         <v>2</v>
       </c>
@@ -2183,10 +2167,10 @@
       <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="24"/>
+      <c r="C3" s="25"/>
       <c r="D3" s="14" t="s">
         <v>8</v>
       </c>
@@ -2195,10 +2179,10 @@
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="24"/>
+      <c r="C4" s="25"/>
       <c r="D4" s="14" t="s">
         <v>5</v>
       </c>
@@ -2207,10 +2191,10 @@
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="25"/>
+      <c r="C5" s="26"/>
       <c r="D5" s="15" t="s">
         <v>11</v>
       </c>
@@ -2231,8 +2215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2333,14 +2317,14 @@
       </c>
     </row>
     <row r="5" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="31">
+      <c r="A5" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="32">
         <v>3</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D5" s="19" t="s">
         <v>6</v>
@@ -2371,10 +2355,10 @@
       </c>
     </row>
     <row r="6" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="30"/>
-      <c r="B6" s="32"/>
+      <c r="A6" s="31"/>
+      <c r="B6" s="33"/>
       <c r="C6" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" s="19" t="s">
         <v>6</v>
@@ -2383,7 +2367,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G6" s="19"/>
       <c r="H6" s="19"/>
@@ -2397,18 +2381,20 @@
       <c r="P6" s="19"/>
       <c r="Q6" s="19"/>
       <c r="R6" s="19"/>
-      <c r="S6" s="19"/>
+      <c r="S6" s="19">
+        <v>1</v>
+      </c>
       <c r="T6" s="19"/>
-      <c r="U6" s="19">
+      <c r="U6" s="23">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="30"/>
-      <c r="B7" s="33"/>
+      <c r="A7" s="31"/>
+      <c r="B7" s="34"/>
       <c r="C7" s="19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D7" s="19" t="s">
         <v>9</v>
@@ -2417,7 +2403,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G7" s="19"/>
       <c r="H7" s="19"/>
@@ -2432,21 +2418,23 @@
       <c r="Q7" s="19"/>
       <c r="R7" s="19"/>
       <c r="S7" s="19"/>
-      <c r="T7" s="19"/>
-      <c r="U7" s="19">
-        <f>U6</f>
+      <c r="T7" s="19">
         <v>1</v>
+      </c>
+      <c r="U7" s="23">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="31">
+      <c r="A8" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="32">
         <v>3</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8" s="21" t="s">
         <v>9</v>
@@ -2473,16 +2461,16 @@
       <c r="R8" s="21"/>
       <c r="S8" s="21"/>
       <c r="T8" s="21"/>
-      <c r="U8" s="21">
-        <f>E7-SUM(G8:T8)</f>
+      <c r="U8" s="23">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="32"/>
-      <c r="B9" s="32"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
       <c r="C9" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D9" s="21" t="s">
         <v>9</v>
@@ -2509,16 +2497,16 @@
       <c r="R9" s="21"/>
       <c r="S9" s="21"/>
       <c r="T9" s="21"/>
-      <c r="U9" s="21">
+      <c r="U9" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="33"/>
-      <c r="B10" s="33"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="34"/>
       <c r="C10" s="21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>6</v>
@@ -2527,7 +2515,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G10" s="21"/>
       <c r="H10" s="21"/>
@@ -2541,22 +2529,24 @@
       <c r="P10" s="21"/>
       <c r="Q10" s="21"/>
       <c r="R10" s="21"/>
-      <c r="S10" s="21"/>
+      <c r="S10" s="21">
+        <v>1</v>
+      </c>
       <c r="T10" s="21"/>
-      <c r="U10" s="22">
+      <c r="U10" s="23">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" s="31">
+      <c r="A11" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="32">
         <v>5</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="19" t="s">
         <v>3</v>
@@ -2581,16 +2571,16 @@
       <c r="R11" s="19"/>
       <c r="S11" s="19"/>
       <c r="T11" s="19"/>
-      <c r="U11" s="22">
+      <c r="U11" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="30"/>
-      <c r="B12" s="32"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="33"/>
       <c r="C12" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" s="19" t="s">
         <v>3</v>
@@ -2617,16 +2607,16 @@
       <c r="R12" s="19"/>
       <c r="S12" s="19"/>
       <c r="T12" s="19"/>
-      <c r="U12" s="22">
-        <f>U11</f>
+      <c r="U12" s="23">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="30"/>
-      <c r="B13" s="33"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="34"/>
       <c r="C13" s="19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D13" s="19" t="s">
         <v>9</v>
@@ -2653,9 +2643,9 @@
       <c r="R13" s="19"/>
       <c r="S13" s="19"/>
       <c r="T13" s="19"/>
-      <c r="U13" s="22">
-        <f>E12-SUM(G13:T13)</f>
-        <v>1</v>
+      <c r="U13" s="23">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
@@ -2723,15 +2713,15 @@
       </c>
       <c r="S14" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T14" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U14" s="2">
         <f t="shared" ref="U14" si="2">E14-SUM(G14:T14)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
@@ -2866,11 +2856,11 @@
       </c>
       <c r="S16" s="2">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T16" s="2">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="U16" s="10"/>
     </row>
@@ -2914,34 +2904,34 @@
     <mergeCell ref="B8:B10"/>
   </mergeCells>
   <conditionalFormatting sqref="U14">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="13" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F10">
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"To do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U5:U13">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11:F13">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"To do"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2971,7 +2961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>

</xml_diff>